<commit_message>
update excela i word s odradjenim zadacima
ako hoces stavi 3.5h meni, ali ne mislim stavljati manje od onog što sam
bio u banci
</commit_message>
<xml_diff>
--- a/NAVA Banka/Zahtjevi za informatiku.xlsx
+++ b/NAVA Banka/Zahtjevi za informatiku.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Documents\NAVA Banka\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>ZAHTJEVI ZA INFORMATIKU</t>
   </si>
@@ -158,12 +158,27 @@
     <t>ARHIVIRATI PODATKE (ABOS, MREŽNI DISK)</t>
   </si>
   <si>
+    <t>Živić</t>
+  </si>
+  <si>
+    <t>Gudelj</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>nema potrebe za backupom (mrežni disk se sastoji od diskova u RAID polju gdje su podaci zaštićeni od kvara pojedinog diska), ABOS backup se vrši na denovnoj bazi na kazetice</t>
+  </si>
+  <si>
     <t xml:space="preserve">partija: 6110001099 Gucek
 partija: 6110000645 Skelin
-+ nove partije: Bratko, Zdunić + Unija industija (otplatni plan/učitanje)
++ nove partije: Bratko, Zdunić + Unija industija (otplatni plan/učitanje) + TPK
 + Farma – neiskorišteni kredit u EUR
 - u otplatnom planu anuitetnog kredita s valutnom klauzulom nakon umanjenja glavnice stanje kredita nije točno;
 - u pregledu aneksa iugovora nije točan iznos kredita </t>
+  </si>
+  <si>
+    <t>srijeda</t>
   </si>
 </sst>
 </file>
@@ -273,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,9 +328,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -324,6 +336,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,42 +631,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="69.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -669,8 +693,12 @@
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="19">
+        <v>42044</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -680,10 +708,14 @@
         <v>11</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="18">
+        <v>42044</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
@@ -721,8 +753,12 @@
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="19">
+        <v>42044</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -735,7 +771,9 @@
         <v>19</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
@@ -771,8 +809,12 @@
         <v>25</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="19">
+        <v>42044</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -782,8 +824,12 @@
         <v>26</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="6"/>
+      <c r="D13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="19">
+        <v>42044</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -793,8 +839,12 @@
         <v>28</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="19">
+        <v>42044</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -804,19 +854,29 @@
         <v>29</v>
       </c>
       <c r="C15" s="7"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="18">
+        <v>42044</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="3"/>
+      <c r="C16" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>